<commit_message>
Added descriptions for structs created and function prototype isValidInput()
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/traceability-matrix-template.xlsx
+++ b/Documents/Testing/TestDocuments/traceability-matrix-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doggy\Documents\Seneca CPA (Local)\SFT221\Final Project\Document Templates, Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D607DC95-71D7-4822-BE84-F79C705CCB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5741D0BA-C523-4470-A624-2D16AA797B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>declare isValidInput()</t>
+  </si>
+  <si>
+    <t>make truck and shipement struct</t>
   </si>
 </sst>
 </file>
@@ -614,14 +620,14 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -706,10 +712,18 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -723,10 +737,18 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1035,10 +1057,13 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="50.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">

</xml_diff>

<commit_message>
Fixed typo in traceability-matrix-template.xlsx. Added macros for max/min values for destination point input in truck.h. Created truck.c file w/preliminary function definition templates.
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/traceability-matrix-template.xlsx
+++ b/Documents/Testing/TestDocuments/traceability-matrix-template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doggy\Documents\Seneca CPA (Local)\SFT221\Final Project\Document Templates, Samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doggy\Documents\Seneca CPA (Local)\SFT221\SFT-Milstone-1\Documents\Testing\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5741D0BA-C523-4470-A624-2D16AA797B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F99AF2-B148-41BA-B5F8-1AB415742B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TrMatrix" sheetId="1" r:id="rId1"/>
     <sheet name="Jira" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -173,25 +173,25 @@
     <t>algo to check if truck is already full (weight and volume)</t>
   </si>
   <si>
-    <t>algo to print out divert in alpha/letter combination (ex. A2)</t>
-  </si>
-  <si>
     <t>application should be able to print out diverted route, if any</t>
   </si>
   <si>
     <t>compile, build, and run</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
     <t>declare isValidInput()</t>
   </si>
   <si>
-    <t>make truck and shipement struct</t>
+    <t>algo to print out divert in number/letter combination (ex. 12A)</t>
+  </si>
+  <si>
+    <t>make truck and shipment struct</t>
+  </si>
+  <si>
+    <t>Test Description/Changes Made</t>
   </si>
 </sst>
 </file>
@@ -283,12 +283,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,10 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,7 +621,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,40 +632,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -681,25 +682,27 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -708,23 +711,25 @@
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -733,23 +738,25 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -758,7 +765,7 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -775,7 +782,7 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -792,7 +799,7 @@
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
@@ -809,7 +816,7 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
@@ -826,7 +833,7 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -843,7 +850,7 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -860,7 +867,7 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
@@ -877,7 +884,7 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
@@ -894,7 +901,7 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
@@ -911,7 +918,7 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
@@ -928,7 +935,7 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
@@ -945,7 +952,7 @@
       <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -962,7 +969,7 @@
       <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
@@ -977,7 +984,7 @@
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
@@ -992,7 +999,7 @@
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
@@ -1007,7 +1014,7 @@
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
@@ -1022,7 +1029,7 @@
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
@@ -1054,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835D6731-823A-430D-8774-F952F0EE7C5C}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,147 +1073,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I14" s="10"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I15" s="10"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="10"/>
+      <c r="A16" s="5"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17" s="10"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>